<commit_message>
new data & fixed backtesters
</commit_message>
<xml_diff>
--- a/results/complete_backtester_medium_20250721_164400.xlsx
+++ b/results/complete_backtester_medium_20250721_164400.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sim\Desktop\Quant\OTC\trading-strategy-automation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A61CCA6-2752-4504-85D0-580FC7A7CD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207FD68D-08D7-433D-BF97-F307BE0F9455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_Results" sheetId="1" r:id="rId1"/>
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N951"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42527,7 +42527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE8D9CF-5C1F-483A-9D71-93C9CFE97C13}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -42821,12 +42821,14 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -43762,9 +43764,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>

</xml_diff>